<commit_message>
+updated: treatment count list in Tab-delimited and MS EXCEL formats --> work-in-progress
</commit_message>
<xml_diff>
--- a/generateMonthlySummaryReport/add-on software/assets/treatmentCountList.xlsx
+++ b/generateMonthlySummaryReport/add-on software/assets/treatmentCountList.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="14">
-  <si>
-    <t> 2017</t>
-  </si>
-  <si>
-    <t> 2018</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="12">
   <si>
     <t>JAN</t>
   </si>
@@ -542,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,12 +579,12 @@
         <v>2016</v>
       </c>
       <c r="R1" s="10"/>
-      <c r="S1" s="5" t="s">
-        <v>0</v>
+      <c r="S1" s="5">
+        <v>2017</v>
       </c>
       <c r="T1" s="15"/>
-      <c r="U1" s="11" t="s">
-        <v>1</v>
+      <c r="U1" s="11">
+        <v>2018</v>
       </c>
       <c r="V1" s="7"/>
       <c r="W1" s="6">
@@ -626,73 +620,73 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="16">
         <v>246</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="16">
         <v>265</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="16">
         <v>251</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H3" s="16">
         <v>213</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J3" s="16">
         <v>231</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L3" s="16">
         <v>134</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N3" s="16">
         <v>148</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P3" s="16">
         <v>349</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R3" s="16">
         <v>199</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T3" s="16">
         <v>119</v>
       </c>
       <c r="U3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V3" s="16">
         <v>238</v>
       </c>
       <c r="W3" s="16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X3" s="16">
         <v>131</v>
@@ -700,73 +694,73 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="16">
         <v>275</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="16">
         <v>311</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="16">
         <v>250</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4" s="16">
         <v>151</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J4" s="16">
         <v>296</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L4" s="16">
         <v>137</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N4" s="16">
         <v>86</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P4" s="16">
         <v>182</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R4" s="16">
         <v>337</v>
       </c>
       <c r="S4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T4" s="16">
         <v>68</v>
       </c>
       <c r="U4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V4" s="16">
         <v>67</v>
       </c>
       <c r="W4" s="16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X4" s="16">
         <v>101</v>
@@ -774,73 +768,73 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="16">
         <v>260</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="16">
         <v>153</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" s="16">
         <v>75</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5" s="16">
         <v>200</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5" s="16">
         <v>208</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L5" s="16">
         <v>168</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N5" s="16">
         <v>103</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P5" s="16">
         <v>140</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R5" s="16">
         <v>212</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T5" s="16">
         <v>340</v>
       </c>
       <c r="U5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V5" s="16">
         <v>113</v>
       </c>
       <c r="W5" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X5" s="16">
         <v>288</v>
@@ -848,73 +842,73 @@
     </row>
     <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="16">
         <v>90</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6" s="16">
         <v>273</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" s="16">
         <v>71</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H6" s="16">
         <v>133</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J6" s="16">
         <v>78</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L6" s="16">
         <v>327</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N6" s="16">
         <v>328</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P6" s="16">
         <v>151</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R6" s="16">
         <v>319</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T6" s="16">
         <v>113</v>
       </c>
       <c r="U6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V6" s="16">
         <v>227</v>
       </c>
       <c r="W6" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X6" s="16">
         <v>287</v>
@@ -922,577 +916,577 @@
     </row>
     <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="16">
         <v>107</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="16">
         <v>234</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7" s="16">
         <v>105</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H7" s="16">
         <v>232</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J7" s="16">
         <v>180</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L7" s="16">
         <v>355</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N7" s="16">
         <v>107</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P7" s="16">
         <v>131</v>
       </c>
       <c r="Q7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R7" s="16">
         <v>199</v>
       </c>
       <c r="S7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T7" s="16">
         <v>78</v>
       </c>
       <c r="U7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V7" s="16">
         <v>302</v>
       </c>
       <c r="W7" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X7" s="16"/>
     </row>
     <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="16">
         <v>359</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" s="16">
         <v>209</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8" s="16">
         <v>351</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H8" s="16">
         <v>243</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J8" s="16">
         <v>84</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L8" s="16">
         <v>351</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N8" s="16">
         <v>337</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P8" s="16">
         <v>91</v>
       </c>
       <c r="Q8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R8" s="16">
         <v>143</v>
       </c>
       <c r="S8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="T8" s="16">
         <v>281</v>
       </c>
       <c r="U8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="V8" s="16">
         <v>258</v>
       </c>
       <c r="W8" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="X8" s="16"/>
     </row>
     <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="16">
         <v>234</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" s="16">
         <v>87</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F9" s="16">
         <v>127</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H9" s="16">
         <v>95</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J9" s="16">
         <v>167</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L9" s="16">
         <v>323</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N9" s="16">
         <v>236</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P9" s="16">
         <v>292</v>
       </c>
       <c r="Q9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="R9" s="16">
         <v>61</v>
       </c>
       <c r="S9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="T9" s="16">
         <v>341</v>
       </c>
       <c r="U9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="V9" s="16">
         <v>120</v>
       </c>
       <c r="W9" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="X9" s="16"/>
     </row>
     <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="16">
         <v>237</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10" s="16">
         <v>168</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F10" s="16">
         <v>183</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H10" s="16">
         <v>241</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J10" s="16">
         <v>154</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L10" s="16">
         <v>190</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N10" s="16">
         <v>342</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P10" s="16">
         <v>331</v>
       </c>
       <c r="Q10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="R10" s="16">
         <v>296</v>
       </c>
       <c r="S10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="T10" s="16">
         <v>61</v>
       </c>
       <c r="U10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="V10" s="16">
         <v>61</v>
       </c>
       <c r="W10" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="X10" s="16"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="16">
         <v>202</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11" s="16">
         <v>344</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F11" s="16">
         <v>357</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H11" s="16">
         <v>233</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J11" s="16">
         <v>332</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L11" s="16">
         <v>117</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N11" s="16">
         <v>149</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P11" s="16">
         <v>235</v>
       </c>
       <c r="Q11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="R11" s="16">
         <v>319</v>
       </c>
       <c r="S11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T11" s="16">
         <v>177</v>
       </c>
       <c r="U11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V11" s="16">
         <v>337</v>
       </c>
       <c r="W11" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="X11" s="16"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="16">
         <v>173</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" s="16">
         <v>357</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F12" s="16">
         <v>269</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H12" s="16">
         <v>164</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J12" s="16">
         <v>113</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L12" s="16">
         <v>158</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N12" s="16">
         <v>354</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P12" s="16">
         <v>131</v>
       </c>
       <c r="Q12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R12" s="16">
         <v>258</v>
       </c>
       <c r="S12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="T12" s="16">
         <v>192</v>
       </c>
       <c r="U12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="V12" s="16">
         <v>75</v>
       </c>
       <c r="W12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X12" s="16"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="16">
         <v>202</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="16">
         <v>85</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F13" s="16">
         <v>79</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H13" s="16">
         <v>253</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J13" s="16">
         <v>230</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L13" s="16">
         <v>295</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N13" s="16">
         <v>355</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P13" s="16">
         <v>314</v>
       </c>
       <c r="Q13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="R13" s="16">
         <v>239</v>
       </c>
       <c r="S13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="T13" s="16">
         <v>226</v>
       </c>
       <c r="U13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V13" s="16">
         <v>221</v>
       </c>
       <c r="W13" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="X13" s="16"/>
     </row>
     <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="16">
         <v>91</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D14" s="16">
         <v>273</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F14" s="16">
         <v>309</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H14" s="16">
         <v>319</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J14" s="16">
         <v>83</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L14" s="16">
         <v>342</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N14" s="16">
         <v>234</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P14" s="16">
         <v>268</v>
       </c>
       <c r="Q14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="R14" s="16">
         <v>269</v>
       </c>
       <c r="S14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="T14" s="16">
         <v>88</v>
       </c>
       <c r="U14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V14" s="16">
         <v>69</v>
       </c>
       <c r="W14" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="X14" s="16"/>
     </row>

</xml_diff>

<commit_message>
+updated: treatment count list assets file --> I've set the treatment count values that are blank/empty to -1. --> Interestingly, this system of setting numerical values to certain objects can be used to make a map built on square tiles, with a grid as the guide. +updated: instructions to process the current/present Monthly Statistics assets file by storing the data in a virtual container --> work-in-progress
</commit_message>
<xml_diff>
--- a/generateMonthlySummaryReport/add-on software/assets/treatmentCountList.xlsx
+++ b/generateMonthlySummaryReport/add-on software/assets/treatmentCountList.xlsx
@@ -536,9 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -984,7 +982,9 @@
       <c r="W7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="X7" s="16"/>
+      <c r="X7" s="16">
+        <v>-1</v>
+      </c>
     </row>
     <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
@@ -1056,7 +1056,9 @@
       <c r="W8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="X8" s="16"/>
+      <c r="X8" s="16">
+        <v>-1</v>
+      </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
@@ -1128,7 +1130,9 @@
       <c r="W9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="X9" s="16"/>
+      <c r="X9" s="16">
+        <v>-1</v>
+      </c>
     </row>
     <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
@@ -1200,7 +1204,9 @@
       <c r="W10" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="X10" s="16"/>
+      <c r="X10" s="16">
+        <v>-1</v>
+      </c>
     </row>
     <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
@@ -1272,7 +1278,9 @@
       <c r="W11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="X11" s="16"/>
+      <c r="X11" s="16">
+        <v>-1</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
@@ -1344,7 +1352,9 @@
       <c r="W12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="X12" s="16"/>
+      <c r="X12" s="16">
+        <v>-1</v>
+      </c>
     </row>
     <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
@@ -1416,7 +1426,9 @@
       <c r="W13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="X13" s="16"/>
+      <c r="X13" s="16">
+        <v>-1</v>
+      </c>
     </row>
     <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
@@ -1488,7 +1500,9 @@
       <c r="W14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="X14" s="16"/>
+      <c r="X14" s="16">
+        <v>-1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>